<commit_message>
update write excel settings
</commit_message>
<xml_diff>
--- a/scrape/mid-uni/output/excel/extracted.xlsx
+++ b/scrape/mid-uni/output/excel/extracted.xlsx
@@ -2269,9 +2269,9 @@
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="3" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="100.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1">
@@ -2304,7 +2304,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="120" customHeight="1">
+    <row r="3" spans="1:6" ht="200" customHeight="1">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="120" customHeight="1">
+    <row r="4" spans="1:6" ht="200" customHeight="1">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="120" customHeight="1">
+    <row r="5" spans="1:6" ht="200" customHeight="1">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="120" customHeight="1">
+    <row r="6" spans="1:6" ht="200" customHeight="1">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="120" customHeight="1">
+    <row r="7" spans="1:6" ht="200" customHeight="1">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="120" customHeight="1">
+    <row r="8" spans="1:6" ht="200" customHeight="1">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="120" customHeight="1">
+    <row r="9" spans="1:6" ht="200" customHeight="1">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="120" customHeight="1">
+    <row r="10" spans="1:6" ht="200" customHeight="1">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="120" customHeight="1">
+    <row r="11" spans="1:6" ht="200" customHeight="1">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="120" customHeight="1">
+    <row r="12" spans="1:6" ht="200" customHeight="1">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="120" customHeight="1">
+    <row r="13" spans="1:6" ht="200" customHeight="1">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="120" customHeight="1">
+    <row r="14" spans="1:6" ht="200" customHeight="1">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="120" customHeight="1">
+    <row r="15" spans="1:6" ht="200" customHeight="1">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="120" customHeight="1">
+    <row r="16" spans="1:6" ht="200" customHeight="1">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="120" customHeight="1">
+    <row r="17" spans="1:6" ht="200" customHeight="1">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="120" customHeight="1">
+    <row r="18" spans="1:6" ht="200" customHeight="1">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="120" customHeight="1">
+    <row r="19" spans="1:6" ht="200" customHeight="1">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="120" customHeight="1">
+    <row r="20" spans="1:6" ht="200" customHeight="1">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="120" customHeight="1">
+    <row r="21" spans="1:6" ht="200" customHeight="1">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="120" customHeight="1">
+    <row r="22" spans="1:6" ht="200" customHeight="1">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="120" customHeight="1">
+    <row r="23" spans="1:6" ht="200" customHeight="1">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="120" customHeight="1">
+    <row r="24" spans="1:6" ht="200" customHeight="1">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="120" customHeight="1">
+    <row r="25" spans="1:6" ht="200" customHeight="1">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="120" customHeight="1">
+    <row r="26" spans="1:6" ht="200" customHeight="1">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="120" customHeight="1">
+    <row r="27" spans="1:6" ht="200" customHeight="1">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="120" customHeight="1">
+    <row r="28" spans="1:6" ht="200" customHeight="1">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="120" customHeight="1">
+    <row r="29" spans="1:6" ht="200" customHeight="1">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="120" customHeight="1">
+    <row r="30" spans="1:6" ht="200" customHeight="1">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="120" customHeight="1">
+    <row r="31" spans="1:6" ht="200" customHeight="1">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="120" customHeight="1">
+    <row r="32" spans="1:6" ht="200" customHeight="1">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="120" customHeight="1">
+    <row r="33" spans="1:6" ht="200" customHeight="1">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="120" customHeight="1">
+    <row r="34" spans="1:6" ht="200" customHeight="1">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="120" customHeight="1">
+    <row r="35" spans="1:6" ht="200" customHeight="1">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="120" customHeight="1">
+    <row r="36" spans="1:6" ht="200" customHeight="1">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="120" customHeight="1">
+    <row r="37" spans="1:6" ht="200" customHeight="1">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="120" customHeight="1">
+    <row r="38" spans="1:6" ht="200" customHeight="1">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="120" customHeight="1">
+    <row r="39" spans="1:6" ht="200" customHeight="1">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="120" customHeight="1">
+    <row r="40" spans="1:6" ht="200" customHeight="1">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="120" customHeight="1">
+    <row r="41" spans="1:6" ht="200" customHeight="1">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="120" customHeight="1">
+    <row r="42" spans="1:6" ht="200" customHeight="1">
       <c r="A42" s="3">
         <v>40</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="120" customHeight="1">
+    <row r="43" spans="1:6" ht="200" customHeight="1">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="120" customHeight="1">
+    <row r="44" spans="1:6" ht="200" customHeight="1">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="120" customHeight="1">
+    <row r="45" spans="1:6" ht="200" customHeight="1">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="120" customHeight="1">
+    <row r="46" spans="1:6" ht="200" customHeight="1">
       <c r="A46" s="3">
         <v>44</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="120" customHeight="1">
+    <row r="47" spans="1:6" ht="200" customHeight="1">
       <c r="A47" s="3">
         <v>45</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="120" customHeight="1">
+    <row r="48" spans="1:6" ht="200" customHeight="1">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="120" customHeight="1">
+    <row r="49" spans="1:6" ht="200" customHeight="1">
       <c r="A49" s="3">
         <v>47</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="120" customHeight="1">
+    <row r="50" spans="1:6" ht="200" customHeight="1">
       <c r="A50" s="3">
         <v>48</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="120" customHeight="1">
+    <row r="51" spans="1:6" ht="200" customHeight="1">
       <c r="A51" s="3">
         <v>49</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="120" customHeight="1">
+    <row r="52" spans="1:6" ht="200" customHeight="1">
       <c r="A52" s="3">
         <v>50</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="120" customHeight="1">
+    <row r="53" spans="1:6" ht="200" customHeight="1">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="120" customHeight="1">
+    <row r="54" spans="1:6" ht="200" customHeight="1">
       <c r="A54" s="3">
         <v>52</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="120" customHeight="1">
+    <row r="55" spans="1:6" ht="200" customHeight="1">
       <c r="A55" s="3">
         <v>53</v>
       </c>
@@ -3346,7 +3346,7 @@
       </c>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:6" ht="120" customHeight="1">
+    <row r="56" spans="1:6" ht="200" customHeight="1">
       <c r="A56" s="3">
         <v>54</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="120" customHeight="1">
+    <row r="57" spans="1:6" ht="200" customHeight="1">
       <c r="A57" s="3">
         <v>55</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="120" customHeight="1">
+    <row r="58" spans="1:6" ht="200" customHeight="1">
       <c r="A58" s="3">
         <v>56</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="120" customHeight="1">
+    <row r="59" spans="1:6" ht="200" customHeight="1">
       <c r="A59" s="3">
         <v>57</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="120" customHeight="1">
+    <row r="60" spans="1:6" ht="200" customHeight="1">
       <c r="A60" s="3">
         <v>58</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="120" customHeight="1">
+    <row r="61" spans="1:6" ht="200" customHeight="1">
       <c r="A61" s="3">
         <v>59</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="120" customHeight="1">
+    <row r="62" spans="1:6" ht="200" customHeight="1">
       <c r="A62" s="3">
         <v>60</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="120" customHeight="1">
+    <row r="63" spans="1:6" ht="200" customHeight="1">
       <c r="A63" s="3">
         <v>61</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="120" customHeight="1">
+    <row r="64" spans="1:6" ht="200" customHeight="1">
       <c r="A64" s="3">
         <v>62</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="120" customHeight="1">
+    <row r="65" spans="1:6" ht="200" customHeight="1">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="120" customHeight="1">
+    <row r="66" spans="1:6" ht="200" customHeight="1">
       <c r="A66" s="3">
         <v>64</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="120" customHeight="1">
+    <row r="67" spans="1:6" ht="200" customHeight="1">
       <c r="A67" s="3">
         <v>65</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="120" customHeight="1">
+    <row r="68" spans="1:6" ht="200" customHeight="1">
       <c r="A68" s="3">
         <v>66</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="120" customHeight="1">
+    <row r="69" spans="1:6" ht="200" customHeight="1">
       <c r="A69" s="3">
         <v>67</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="120" customHeight="1">
+    <row r="70" spans="1:6" ht="200" customHeight="1">
       <c r="A70" s="3">
         <v>68</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="120" customHeight="1">
+    <row r="71" spans="1:6" ht="200" customHeight="1">
       <c r="A71" s="3">
         <v>69</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="120" customHeight="1">
+    <row r="72" spans="1:6" ht="200" customHeight="1">
       <c r="A72" s="3">
         <v>70</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="120" customHeight="1">
+    <row r="73" spans="1:6" ht="200" customHeight="1">
       <c r="A73" s="3">
         <v>71</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="120" customHeight="1">
+    <row r="74" spans="1:6" ht="200" customHeight="1">
       <c r="A74" s="3">
         <v>72</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="120" customHeight="1">
+    <row r="75" spans="1:6" ht="200" customHeight="1">
       <c r="A75" s="3">
         <v>73</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="120" customHeight="1">
+    <row r="76" spans="1:6" ht="200" customHeight="1">
       <c r="A76" s="3">
         <v>74</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="120" customHeight="1">
+    <row r="77" spans="1:6" ht="200" customHeight="1">
       <c r="A77" s="3">
         <v>75</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="120" customHeight="1">
+    <row r="78" spans="1:6" ht="200" customHeight="1">
       <c r="A78" s="3">
         <v>76</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="120" customHeight="1">
+    <row r="79" spans="1:6" ht="200" customHeight="1">
       <c r="A79" s="3">
         <v>77</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="120" customHeight="1">
+    <row r="80" spans="1:6" ht="200" customHeight="1">
       <c r="A80" s="3">
         <v>78</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="120" customHeight="1">
+    <row r="81" spans="1:6" ht="200" customHeight="1">
       <c r="A81" s="3">
         <v>79</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="120" customHeight="1">
+    <row r="82" spans="1:6" ht="200" customHeight="1">
       <c r="A82" s="3">
         <v>80</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="120" customHeight="1">
+    <row r="83" spans="1:6" ht="200" customHeight="1">
       <c r="A83" s="3">
         <v>81</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="120" customHeight="1">
+    <row r="84" spans="1:6" ht="200" customHeight="1">
       <c r="A84" s="3">
         <v>82</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="120" customHeight="1">
+    <row r="85" spans="1:6" ht="200" customHeight="1">
       <c r="A85" s="3">
         <v>83</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="120" customHeight="1">
+    <row r="86" spans="1:6" ht="200" customHeight="1">
       <c r="A86" s="3">
         <v>84</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="120" customHeight="1">
+    <row r="87" spans="1:6" ht="200" customHeight="1">
       <c r="A87" s="3">
         <v>85</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="120" customHeight="1">
+    <row r="88" spans="1:6" ht="200" customHeight="1">
       <c r="A88" s="3">
         <v>86</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="120" customHeight="1">
+    <row r="89" spans="1:6" ht="200" customHeight="1">
       <c r="A89" s="3">
         <v>87</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="120" customHeight="1">
+    <row r="90" spans="1:6" ht="200" customHeight="1">
       <c r="A90" s="3">
         <v>88</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="120" customHeight="1">
+    <row r="91" spans="1:6" ht="200" customHeight="1">
       <c r="A91" s="3">
         <v>89</v>
       </c>
@@ -4030,7 +4030,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="120" customHeight="1">
+    <row r="92" spans="1:6" ht="200" customHeight="1">
       <c r="A92" s="3">
         <v>90</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="120" customHeight="1">
+    <row r="93" spans="1:6" ht="200" customHeight="1">
       <c r="A93" s="3">
         <v>91</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="120" customHeight="1">
+    <row r="94" spans="1:6" ht="200" customHeight="1">
       <c r="A94" s="3">
         <v>92</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="120" customHeight="1">
+    <row r="95" spans="1:6" ht="200" customHeight="1">
       <c r="A95" s="3">
         <v>93</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="120" customHeight="1">
+    <row r="96" spans="1:6" ht="200" customHeight="1">
       <c r="A96" s="3">
         <v>94</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="120" customHeight="1">
+    <row r="97" spans="1:6" ht="200" customHeight="1">
       <c r="A97" s="3">
         <v>95</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="120" customHeight="1">
+    <row r="98" spans="1:6" ht="200" customHeight="1">
       <c r="A98" s="3">
         <v>96</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="120" customHeight="1">
+    <row r="99" spans="1:6" ht="200" customHeight="1">
       <c r="A99" s="3">
         <v>97</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="120" customHeight="1">
+    <row r="100" spans="1:6" ht="200" customHeight="1">
       <c r="A100" s="3">
         <v>98</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="120" customHeight="1">
+    <row r="101" spans="1:6" ht="200" customHeight="1">
       <c r="A101" s="3">
         <v>99</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="120" customHeight="1">
+    <row r="102" spans="1:6" ht="200" customHeight="1">
       <c r="A102" s="3">
         <v>100</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="120" customHeight="1">
+    <row r="103" spans="1:6" ht="200" customHeight="1">
       <c r="A103" s="3">
         <v>101</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="120" customHeight="1">
+    <row r="104" spans="1:6" ht="200" customHeight="1">
       <c r="A104" s="3">
         <v>102</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="120" customHeight="1">
+    <row r="105" spans="1:6" ht="200" customHeight="1">
       <c r="A105" s="3">
         <v>103</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="120" customHeight="1">
+    <row r="106" spans="1:6" ht="200" customHeight="1">
       <c r="A106" s="3">
         <v>104</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="120" customHeight="1">
+    <row r="107" spans="1:6" ht="200" customHeight="1">
       <c r="A107" s="3">
         <v>105</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="120" customHeight="1">
+    <row r="108" spans="1:6" ht="200" customHeight="1">
       <c r="A108" s="3">
         <v>106</v>
       </c>
@@ -4350,7 +4350,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="120" customHeight="1">
+    <row r="109" spans="1:6" ht="200" customHeight="1">
       <c r="A109" s="3">
         <v>107</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="120" customHeight="1">
+    <row r="110" spans="1:6" ht="200" customHeight="1">
       <c r="A110" s="3">
         <v>108</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="120" customHeight="1">
+    <row r="111" spans="1:6" ht="200" customHeight="1">
       <c r="A111" s="3">
         <v>109</v>
       </c>
@@ -4410,7 +4410,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="120" customHeight="1">
+    <row r="112" spans="1:6" ht="200" customHeight="1">
       <c r="A112" s="3">
         <v>110</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="120" customHeight="1">
+    <row r="113" spans="1:6" ht="200" customHeight="1">
       <c r="A113" s="3">
         <v>111</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="120" customHeight="1">
+    <row r="114" spans="1:6" ht="200" customHeight="1">
       <c r="A114" s="3">
         <v>112</v>
       </c>
@@ -4470,7 +4470,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="120" customHeight="1">
+    <row r="115" spans="1:6" ht="200" customHeight="1">
       <c r="A115" s="3">
         <v>113</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="120" customHeight="1">
+    <row r="116" spans="1:6" ht="200" customHeight="1">
       <c r="A116" s="3">
         <v>114</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="120" customHeight="1">
+    <row r="117" spans="1:6" ht="200" customHeight="1">
       <c r="A117" s="3">
         <v>115</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="120" customHeight="1">
+    <row r="118" spans="1:6" ht="200" customHeight="1">
       <c r="A118" s="3">
         <v>116</v>
       </c>
@@ -4550,7 +4550,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="120" customHeight="1">
+    <row r="119" spans="1:6" ht="200" customHeight="1">
       <c r="A119" s="3">
         <v>117</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="120" customHeight="1">
+    <row r="120" spans="1:6" ht="200" customHeight="1">
       <c r="A120" s="3">
         <v>118</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="120" customHeight="1">
+    <row r="121" spans="1:6" ht="200" customHeight="1">
       <c r="A121" s="3">
         <v>119</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="120" customHeight="1">
+    <row r="122" spans="1:6" ht="200" customHeight="1">
       <c r="A122" s="3">
         <v>120</v>
       </c>
@@ -4630,7 +4630,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="120" customHeight="1">
+    <row r="123" spans="1:6" ht="200" customHeight="1">
       <c r="A123" s="3">
         <v>121</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="120" customHeight="1">
+    <row r="124" spans="1:6" ht="200" customHeight="1">
       <c r="A124" s="3">
         <v>122</v>
       </c>
@@ -4668,7 +4668,7 @@
       </c>
       <c r="F124" s="3"/>
     </row>
-    <row r="125" spans="1:6" ht="120" customHeight="1">
+    <row r="125" spans="1:6" ht="200" customHeight="1">
       <c r="A125" s="3">
         <v>123</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="120" customHeight="1">
+    <row r="126" spans="1:6" ht="200" customHeight="1">
       <c r="A126" s="3">
         <v>124</v>
       </c>
@@ -4708,7 +4708,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="120" customHeight="1">
+    <row r="127" spans="1:6" ht="200" customHeight="1">
       <c r="A127" s="3">
         <v>125</v>
       </c>
@@ -4728,7 +4728,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="120" customHeight="1">
+    <row r="128" spans="1:6" ht="200" customHeight="1">
       <c r="A128" s="3">
         <v>126</v>
       </c>
@@ -4748,7 +4748,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="120" customHeight="1">
+    <row r="129" spans="1:6" ht="200" customHeight="1">
       <c r="A129" s="3">
         <v>127</v>
       </c>
@@ -4768,7 +4768,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="120" customHeight="1">
+    <row r="130" spans="1:6" ht="200" customHeight="1">
       <c r="A130" s="3">
         <v>128</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="120" customHeight="1">
+    <row r="131" spans="1:6" ht="200" customHeight="1">
       <c r="A131" s="3">
         <v>129</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="120" customHeight="1">
+    <row r="132" spans="1:6" ht="200" customHeight="1">
       <c r="A132" s="3">
         <v>130</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="120" customHeight="1">
+    <row r="133" spans="1:6" ht="200" customHeight="1">
       <c r="A133" s="3">
         <v>131</v>
       </c>
@@ -4848,7 +4848,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="120" customHeight="1">
+    <row r="134" spans="1:6" ht="200" customHeight="1">
       <c r="A134" s="3">
         <v>132</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="120" customHeight="1">
+    <row r="135" spans="1:6" ht="200" customHeight="1">
       <c r="A135" s="3">
         <v>133</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="120" customHeight="1">
+    <row r="136" spans="1:6" ht="200" customHeight="1">
       <c r="A136" s="3">
         <v>134</v>
       </c>

</xml_diff>